<commit_message>
f/abaird-sleep: adding nervous validation
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/NervousValidation.xlsx
+++ b/share/doc/validation/Scenarios/NervousValidation.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core\share\doc\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BioGearsResearch\sleep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="-216" windowWidth="20016" windowHeight="7992" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="-210" windowWidth="20010" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="3" r:id="rId2"/>
     <sheet name="Baroreceptors" sheetId="2" r:id="rId3"/>
-    <sheet name="TBI" sheetId="4" r:id="rId4"/>
+    <sheet name="Sleep" sheetId="5" r:id="rId4"/>
+    <sheet name="TBI" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Baroreceptors!$B$2:$L$4</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="76">
   <si>
     <t xml:space="preserve">Scenario </t>
   </si>
@@ -212,6 +213,48 @@
   </si>
   <si>
     <t>Slight increase, remain &lt; 100 @cite gutierrez2004clinical</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Sleep of 4hr per day for 5 days</t>
+  </si>
+  <si>
+    <t>Sampled Scenario Time (min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleep deprivation study taken from spiegle, given carb rich meal (62%) every 5h </t>
+  </si>
+  <si>
+    <t>40% lower (1.42%/min compared to 2.4%/min @cite gutierrez2004clinical</t>
+  </si>
+  <si>
+    <t>Glucose clearance (%/min)</t>
+  </si>
+  <si>
+    <t>Glucose effectiveness (%/min) clearance without insulin</t>
+  </si>
+  <si>
+    <t>Decrease 30% @cite Hosomi1979effect @cite Ottesen2004applied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insulin response (pmol/min) </t>
+  </si>
+  <si>
+    <t>Decrease from 432 to 304 pmol/min @cite Hosomi1979effect @cite Ottesen2004applied</t>
+  </si>
+  <si>
+    <t>Stanford sleepyness score (unitless)</t>
+  </si>
+  <si>
+    <t>Increase from 2.1 to 4.4 @cite Hosomi1979effect @cite Ottesen2004applied</t>
+  </si>
+  <si>
+    <t>Cerebral glucose uptake (% from baseline)</t>
+  </si>
+  <si>
+    <t>Decrease of 7% @cite Hosomi1979effect @cite Ottesen2004applied</t>
   </si>
 </sst>
 </file>
@@ -1249,23 +1292,23 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="30" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="30" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="30"/>
-    <col min="12" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="1.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="30" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="30"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>9</v>
       </c>
@@ -1300,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>9</v>
       </c>
@@ -1335,7 +1378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>9</v>
       </c>
@@ -1437,39 +1480,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
@@ -1491,14 +1534,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -1509,7 +1552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1520,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -1531,7 +1574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
@@ -1542,7 +1585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -1565,35 +1608,35 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="2" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" style="4" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="20" width="9.109375" style="4"/>
-    <col min="21" max="21" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="4"/>
+    <col min="11" max="11" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="20" width="9.140625" style="4"/>
+    <col min="21" max="21" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1675,7 +1718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1728,38 +1771,245 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.140625" customWidth="1"/>
+    <col min="16" max="16" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9">
+        <v>7200</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" style="27" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="27" customWidth="1"/>
     <col min="14" max="14" width="23" style="27" customWidth="1"/>
-    <col min="15" max="15" width="8.5546875" style="27" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="27" customWidth="1"/>
     <col min="16" max="16" width="23" style="27" customWidth="1"/>
-    <col min="17" max="17" width="9.88671875" style="27" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="27" customWidth="1"/>
     <col min="18" max="18" width="23" style="27" customWidth="1"/>
-    <col min="19" max="19" width="2.5546875" customWidth="1"/>
-    <col min="20" max="20" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.5703125" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>41</v>
@@ -1784,7 +2034,7 @@
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
     </row>
-    <row r="2" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1843,7 +2093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1902,7 +2152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1961,7 +2211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2020,7 +2270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2079,7 +2329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2138,7 +2388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2197,7 +2447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L9" s="27" t="s">
         <v>59</v>
       </c>
@@ -2208,18 +2458,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2337,14 +2587,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6320210A-C44C-4B82-8349-5A58CB3B5A77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2355,6 +2597,14 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>